<commit_message>
update Junction, cornstover biorefinery bugs, and biosteam version
</commit_message>
<xml_diff>
--- a/biorefineries/biorefineries/cornstover/_humbird2011.xlsx
+++ b/biorefineries/biorefineries/cornstover/_humbird2011.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoelr\OneDrive\Code\biosteam\biosteam\biorefineries\cornstover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoelr\OneDrive\Code\Bioindustrial-Park\biorefineries\biorefineries\cornstover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{B835EC96-4757-407F-879E-2A46AD6388AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{802D7A91-D58F-4049-A7A5-29F2BF44651F}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B835EC96-4757-407F-879E-2A46AD6388AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{19D2432C-4B2E-48F2-9FD9-AB7B182C570A}"/>
   <bookViews>
-    <workbookView xWindow="1002" yWindow="1498" windowWidth="11635" windowHeight="10137" xr2:uid="{3188A448-B3F0-4EEE-A6DF-294BE8E476D0}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{3188A448-B3F0-4EEE-A6DF-294BE8E476D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,8 +649,8 @@
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O6" sqref="O6"/>
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>